<commit_message>
fis ETL / fix SQL
</commit_message>
<xml_diff>
--- a/Data/Original/comunas.xlsx
+++ b/Data/Original/comunas.xlsx
@@ -81,7 +81,7 @@
     <t>CONSTITUCION - MONTSERRAT - PUERTO MADERO - RETIRO - SAN NICOLAS - SAN TELMO</t>
   </si>
   <si>
-    <t>BELGRANO - COLEGIALES - NUÃ‘EZ</t>
+    <t>BELGRANO - COLEGIALES - NUÑEZ</t>
   </si>
 </sst>
 </file>
@@ -115,11 +115,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -336,7 +339,11 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="5" width="10.71"/>
+    <col customWidth="1" min="1" max="1" width="10.71"/>
+    <col customWidth="1" min="2" max="2" width="17.86"/>
+    <col customWidth="1" min="3" max="3" width="9.0"/>
+    <col customWidth="1" min="4" max="4" width="80.29"/>
+    <col customWidth="1" min="5" max="5" width="14.86"/>
     <col customWidth="1" min="6" max="6" width="22.86"/>
     <col customWidth="1" min="7" max="26" width="10.71"/>
   </cols>
@@ -651,7 +658,7 @@
       <c r="C16" s="1">
         <v>13.0</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E16" s="1">

</xml_diff>